<commit_message>
Reworked support value on association rule/frequent itemset analysis. Also cleaned plotting a little.
</commit_message>
<xml_diff>
--- a/src/data/cwe-rules-filtered/communication_cwe_filtered.xlsx
+++ b/src/data/cwe-rules-filtered/communication_cwe_filtered.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
   <si>
     <t>antecedents</t>
   </si>
@@ -37,34 +37,67 @@
     <t>conviction</t>
   </si>
   <si>
-    <t>frozenset({'CWE-276', 'CWE-200', 'CWE-532'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-327', 'CWE-276', 'CWE-200', 'CWE-532'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-276', 'CWE-200'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-312', 'CWE-532', 'CWE-89'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-276', 'CWE-327'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-312', 'CWE-327', 'CWE-89'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-312', 'CWE-89'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-312', 'CWE-327', 'CWE-532', 'CWE-89'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-276', 'CWE-200', 'CWE-327'})</t>
-  </si>
-  <si>
-    <t>frozenset({'CWE-312', 'CWE-330', 'CWE-532', 'CWE-89'})</t>
+    <t>antecedent_len</t>
+  </si>
+  <si>
+    <t>consequent_len</t>
+  </si>
+  <si>
+    <t>combo_len</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-330', 'CWE-89'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-330', 'CWE-89', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-89'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-89', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-200'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-330'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-200', 'CWE-532'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532', 'CWE-89', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532', 'CWE-89'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-330', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532', 'CWE-330', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532', 'CWE-330'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-532', 'CWE-330', 'CWE-89'})</t>
+  </si>
+  <si>
+    <t>frozenset({'CWE-200', 'CWE-327'})</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -422,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,120 +483,974 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>0.9759036144578314</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F2">
+        <v>0.02351574974597181</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F3">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>0.6024096385542169</v>
-      </c>
-      <c r="D2">
-        <v>0.8771929824561404</v>
-      </c>
-      <c r="E2">
-        <v>1.277316097260696</v>
-      </c>
-      <c r="F2">
-        <v>0.1307882130933373</v>
-      </c>
-      <c r="G2">
-        <v>2.550774526678143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F4">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
-        <v>0.6024096385542169</v>
-      </c>
-      <c r="D3">
-        <v>0.8771929824561404</v>
-      </c>
-      <c r="E3">
-        <v>1.277316097260696</v>
-      </c>
-      <c r="F3">
-        <v>0.1307882130933373</v>
-      </c>
-      <c r="G3">
-        <v>2.550774526678143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>0.8313253012048193</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F5">
+        <v>0.02003193496879074</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
-        <v>0.6024096385542169</v>
-      </c>
-      <c r="D4">
-        <v>0.8771929824561404</v>
-      </c>
-      <c r="E4">
-        <v>1.277316097260696</v>
-      </c>
-      <c r="F4">
-        <v>0.1307882130933373</v>
-      </c>
-      <c r="G4">
-        <v>2.550774526678143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6">
+        <v>0.8313253012048193</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F6">
+        <v>0.02003193496879074</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0.8313253012048193</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F7">
+        <v>0.02003193496879074</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>0.6024096385542169</v>
-      </c>
-      <c r="D5">
-        <v>0.8771929824561404</v>
-      </c>
-      <c r="E5">
-        <v>1.277316097260696</v>
-      </c>
-      <c r="F5">
-        <v>0.1307882130933373</v>
-      </c>
-      <c r="G5">
-        <v>2.550774526678143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F8">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
-        <v>0.6265060240963856</v>
-      </c>
-      <c r="D6">
-        <v>0.8253968253968255</v>
-      </c>
-      <c r="E6">
-        <v>1.223356009070295</v>
-      </c>
-      <c r="F6">
-        <v>0.1143852518507767</v>
-      </c>
-      <c r="G6">
-        <v>1.863088718510406</v>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>0.9036144578313252</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F9">
+        <v>0.02177384235738133</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F10">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F11">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0.9036144578313252</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F12">
+        <v>0.02177384235738133</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D13">
+        <v>0.9710144927536232</v>
+      </c>
+      <c r="E13">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F13">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G13">
+        <v>3.325301204819287</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D14">
+        <v>0.9710144927536232</v>
+      </c>
+      <c r="E14">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F14">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G14">
+        <v>3.325301204819287</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D15">
+        <v>0.9710144927536232</v>
+      </c>
+      <c r="E15">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F15">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G15">
+        <v>3.325301204819287</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D16">
+        <v>0.9710144927536232</v>
+      </c>
+      <c r="E16">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F16">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G16">
+        <v>3.325301204819287</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D17">
+        <v>0.9710144927536232</v>
+      </c>
+      <c r="E17">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F17">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G17">
+        <v>3.325301204819287</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D18">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="E18">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F18">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G18">
+        <v>1.581325301204819</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D19">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="E19">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F19">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G19">
+        <v>1.581325301204819</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D20">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="E20">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F20">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G20">
+        <v>1.581325301204819</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D21">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="E21">
+        <v>1.074589371980676</v>
+      </c>
+      <c r="F21">
+        <v>0.05603135433299467</v>
+      </c>
+      <c r="G21">
+        <v>1.581325301204819</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>0.9036144578313252</v>
+      </c>
+      <c r="D22">
+        <v>0.925925925925926</v>
+      </c>
+      <c r="E22">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F22">
+        <v>0.02177384235738133</v>
+      </c>
+      <c r="G22">
+        <v>1.301204819277108</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>0.9036144578313252</v>
+      </c>
+      <c r="D23">
+        <v>0.925925925925926</v>
+      </c>
+      <c r="E23">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F23">
+        <v>0.02177384235738133</v>
+      </c>
+      <c r="G23">
+        <v>1.301204819277108</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>0.9036144578313252</v>
+      </c>
+      <c r="D24">
+        <v>0.925925925925926</v>
+      </c>
+      <c r="E24">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F24">
+        <v>0.02177384235738133</v>
+      </c>
+      <c r="G24">
+        <v>1.301204819277108</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>0.8313253012048193</v>
+      </c>
+      <c r="D25">
+        <v>0.8518518518518519</v>
+      </c>
+      <c r="E25">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F25">
+        <v>0.02003193496879074</v>
+      </c>
+      <c r="G25">
+        <v>1.13855421686747</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>0.8313253012048193</v>
+      </c>
+      <c r="D26">
+        <v>0.8518518518518519</v>
+      </c>
+      <c r="E26">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F26">
+        <v>0.02003193496879074</v>
+      </c>
+      <c r="G26">
+        <v>1.13855421686747</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D27">
+        <v>0.8271604938271605</v>
+      </c>
+      <c r="E27">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F27">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G27">
+        <v>1.115318416523235</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D28">
+        <v>0.8271604938271605</v>
+      </c>
+      <c r="E28">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F28">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G28">
+        <v>1.115318416523235</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D29">
+        <v>0.8271604938271605</v>
+      </c>
+      <c r="E29">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F29">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G29">
+        <v>1.115318416523235</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D30">
+        <v>0.8271604938271605</v>
+      </c>
+      <c r="E30">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F30">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G30">
+        <v>1.115318416523235</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>0.8072289156626506</v>
+      </c>
+      <c r="D31">
+        <v>0.8271604938271605</v>
+      </c>
+      <c r="E31">
+        <v>1.024691358024691</v>
+      </c>
+      <c r="F31">
+        <v>0.01945129917259392</v>
+      </c>
+      <c r="G31">
+        <v>1.115318416523235</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>